<commit_message>
Spec battery capacity update
</commit_message>
<xml_diff>
--- a/FEASIBILITY STUDY/Spec combined.xlsx
+++ b/FEASIBILITY STUDY/Spec combined.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\L2-DESIGN\FEASIBILITY STUDY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CAC1EC-0B81-4179-A41E-A4F17BCEA5B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E19096F-E1FF-410D-9341-7209C38AD727}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18220" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>User specification</t>
   </si>
@@ -132,9 +132,6 @@
     <t>12S</t>
   </si>
   <si>
-    <t>370Wh</t>
-  </si>
-  <si>
     <t>Depth of discharge</t>
   </si>
   <si>
@@ -169,6 +166,12 @@
   </si>
   <si>
     <t>Wh</t>
+  </si>
+  <si>
+    <t>180Wh</t>
+  </si>
+  <si>
+    <t>est</t>
   </si>
 </sst>
 </file>
@@ -591,15 +594,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252F1252-14C0-49E7-AD01-36C0826662BC}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="41" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -662,15 +666,15 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>13</v>
@@ -686,10 +690,10 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -708,10 +712,10 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -722,48 +726,63 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="9">
         <v>0.9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19">
+        <f>180/0.9</f>
+        <v>200</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B19">
-        <f>370/0.9</f>
-        <v>411.11111111111109</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="B20">
+        <f>2*90*46*158*10^-9 * 10^3</f>
+        <v>1.3082400000000001</v>
+      </c>
+      <c r="C20">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B20">
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="B21">
+        <f>1242*2*10^-3</f>
+        <v>2.484</v>
+      </c>
+      <c r="C21">
         <v>2.7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>